<commit_message>
Descripción de los cambios realizados
</commit_message>
<xml_diff>
--- a/static/exports/diagnosticos_estudiantes.xlsx
+++ b/static/exports/diagnosticos_estudiantes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,6 +1135,122 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Costa</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Urbana</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>VI</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>tarde</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>37</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>alto</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>A menudo</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>A menudo</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Casi nunca</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Casi nunca</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>A menudo</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>Casi nunca Casi nunca</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>De vez en cuando</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>